<commit_message>
adjust order of slimes
</commit_message>
<xml_diff>
--- a/__data__/monster_data_analysis.xlsx
+++ b/__data__/monster_data_analysis.xlsx
@@ -130,31 +130,31 @@
     <t>Knight B</t>
   </si>
   <si>
+    <t>Green Slime A</t>
+  </si>
+  <si>
+    <t>Vampire Bat B</t>
+  </si>
+  <si>
+    <t>Magician B</t>
+  </si>
+  <si>
+    <t>Magician A</t>
+  </si>
+  <si>
+    <t>Magic Sergeant B</t>
+  </si>
+  <si>
+    <t>Dark Knight B</t>
+  </si>
+  <si>
+    <t>Gate-Keeper A</t>
+  </si>
+  <si>
+    <t>Red Slime A</t>
+  </si>
+  <si>
     <t>Slimelord</t>
-  </si>
-  <si>
-    <t>Vampire Bat B</t>
-  </si>
-  <si>
-    <t>Magician B</t>
-  </si>
-  <si>
-    <t>Magician A</t>
-  </si>
-  <si>
-    <t>Magic Sergeant B</t>
-  </si>
-  <si>
-    <t>Dark Knight B</t>
-  </si>
-  <si>
-    <t>Gate-Keeper A</t>
-  </si>
-  <si>
-    <t>Green Slime A</t>
-  </si>
-  <si>
-    <t>Red Slime A</t>
   </si>
   <si>
     <t>Dark Priest</t>
@@ -253,12 +253,18 @@
       <name val="宋体"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+        <bgColor auto="1"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -271,16 +277,16 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="9"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -297,13 +303,13 @@
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -323,6 +329,7 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
+      <rgbColor rgb="ffffffff"/>
       <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
@@ -522,17 +529,17 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -560,10 +567,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -811,12 +818,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
             <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1103,7 +1110,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1131,10 +1138,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">

</xml_diff>